<commit_message>
Code clean up, new way to create characters
</commit_message>
<xml_diff>
--- a/EmotionRegulation/EmotionRegulationAsset/Results/Agreeableness.xlsx
+++ b/EmotionRegulation/EmotionRegulationAsset/Results/Agreeableness.xlsx
@@ -6,13 +6,13 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Sheet1" sheetId="1" r:id="R6db8b502a3fc491b"/>
+    <x:sheet name="Sheet1" sheetId="1" r:id="R0e257455e1b8488a"/>
   </x:sheets>
 </x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <x:si>
     <x:t xml:space="preserve">MOOD     </x:t>
   </x:si>
@@ -44,15 +44,18 @@
     <x:t>Talk</x:t>
   </x:si>
   <x:si>
+    <x:t>Attention Deployment</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Love</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Hello</x:t>
+  </x:si>
+  <x:si>
     <x:t>None</x:t>
   </x:si>
   <x:si>
-    <x:t>Love</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Hello</x:t>
-  </x:si>
-  <x:si>
     <x:t>Conversation</x:t>
   </x:si>
   <x:si>
@@ -77,24 +80,15 @@
     <x:t>Fired</x:t>
   </x:si>
   <x:si>
+    <x:t>Cognitive Change</x:t>
+  </x:si>
+  <x:si>
     <x:t>Crash</x:t>
   </x:si>
   <x:si>
     <x:t>Profits</x:t>
   </x:si>
   <x:si>
-    <x:t>Remorse</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Fly</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Pitty</x:t>
-  </x:si>
-  <x:si>
-    <x:t>BecomeRich</x:t>
-  </x:si>
-  <x:si>
     <x:t>Low Conscientiousness</x:t>
   </x:si>
   <x:si>
@@ -110,7 +104,19 @@
     <x:t>Low Openness</x:t>
   </x:si>
   <x:si>
+    <x:t>[Situation Selection, Weakly]</x:t>
+  </x:si>
+  <x:si>
     <x:t>[Situation Modification, Weakly]</x:t>
+  </x:si>
+  <x:si>
+    <x:t>[Attention Deployment, Strongly]</x:t>
+  </x:si>
+  <x:si>
+    <x:t>[Cognitive Change, Strongly]</x:t>
+  </x:si>
+  <x:si>
+    <x:t>[Response Modulation, Lightly]</x:t>
   </x:si>
   <x:si>
     <x:t>Agreeableness</x:t>
@@ -444,7 +450,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <x:dimension ref="A1:H20"/>
+  <x:dimension ref="A1:H22"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
@@ -478,13 +484,13 @@
     </x:row>
     <x:row r="2">
       <x:c r="A2">
-        <x:v>-1.4827710390090942</x:v>
+        <x:v>-0.7413855195045471</x:v>
       </x:c>
       <x:c r="B2" t="s">
         <x:v>8</x:v>
       </x:c>
       <x:c r="C2">
-        <x:v>4.774208068847656</x:v>
+        <x:v>2.387104034423828</x:v>
       </x:c>
       <x:c r="D2" t="s">
         <x:v>9</x:v>
@@ -495,101 +501,101 @@
     </x:row>
     <x:row r="3">
       <x:c r="A3">
-        <x:v>-0.974892795085907</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="B3" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="C3">
-        <x:v>1.5804238319396973</x:v>
+        <x:v>1.7927955389022827</x:v>
       </x:c>
       <x:c r="D3" t="s">
         <x:v>12</x:v>
       </x:c>
       <x:c r="E3" t="s">
-        <x:v>10</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="4">
       <x:c r="A4">
-        <x:v>0</x:v>
+        <x:v>0.8303518295288086</x:v>
       </x:c>
       <x:c r="B4" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="C4">
-        <x:v>2.3942959308624268</x:v>
+        <x:v>2.6735565662384033</x:v>
       </x:c>
       <x:c r="D4" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E4" t="s">
         <x:v>13</x:v>
-      </x:c>
-      <x:c r="E4" t="s">
-        <x:v>10</x:v>
       </x:c>
     </x:row>
     <x:row r="5">
       <x:c r="A5">
-        <x:v>1.4531155824661255</x:v>
+        <x:v>2.3478033542633057</x:v>
       </x:c>
       <x:c r="B5" t="s">
         <x:v>11</x:v>
       </x:c>
       <x:c r="C5">
-        <x:v>4.6787238121032715</x:v>
+        <x:v>4.9165802001953125</x:v>
       </x:c>
       <x:c r="D5" t="s">
-        <x:v>14</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E5" t="s">
-        <x:v>10</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="6">
       <x:c r="A6">
-        <x:v>0</x:v>
+        <x:v>1.046940803527832</x:v>
       </x:c>
       <x:c r="B6" t="s">
         <x:v>8</x:v>
       </x:c>
       <x:c r="C6">
-        <x:v>4.357959747314453</x:v>
+        <x:v>4.1016740798950195</x:v>
       </x:c>
       <x:c r="D6" t="s">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="E6" t="s">
-        <x:v>10</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="7">
       <x:c r="A7">
-        <x:v>0.5931084156036377</x:v>
+        <x:v>1.7211663722991943</x:v>
       </x:c>
       <x:c r="B7" t="s">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="C7">
-        <x:v>1.9096832275390625</x:v>
+        <x:v>2.2095818519592285</x:v>
       </x:c>
       <x:c r="D7" t="s">
-        <x:v>17</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="E7" t="s">
-        <x:v>10</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="8">
       <x:c r="A8">
-        <x:v>-0.8437083959579468</x:v>
+        <x:v>0.7149765491485596</x:v>
       </x:c>
       <x:c r="B8" t="s">
         <x:v>8</x:v>
       </x:c>
       <x:c r="C8">
-        <x:v>4.604310512542725</x:v>
+        <x:v>3.1760647296905518</x:v>
       </x:c>
       <x:c r="D8" t="s">
-        <x:v>18</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="E8" t="s">
         <x:v>10</x:v>
@@ -597,87 +603,63 @@
     </x:row>
     <x:row r="9">
       <x:c r="A9">
-        <x:v>-2.5697827339172363</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="B9" t="s">
-        <x:v>19</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="C9">
-        <x:v>5.588795185089111</x:v>
+        <x:v>2.5324015617370605</x:v>
       </x:c>
       <x:c r="D9" t="s">
-        <x:v>20</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="E9" t="s">
-        <x:v>10</x:v>
+        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="10">
       <x:c r="A10">
-        <x:v>-4.637181282043457</x:v>
+        <x:v>-0.5182909965515137</x:v>
       </x:c>
       <x:c r="B10" t="s">
-        <x:v>19</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="C10">
-        <x:v>6.751622676849365</x:v>
+        <x:v>1.6687870025634766</x:v>
       </x:c>
       <x:c r="D10" t="s">
-        <x:v>21</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="E10" t="s">
-        <x:v>10</x:v>
+        <x:v>22</x:v>
       </x:c>
     </x:row>
     <x:row r="11">
       <x:c r="A11">
-        <x:v>-2.624037742614746</x:v>
+        <x:v>1.8139854669570923</x:v>
       </x:c>
       <x:c r="B11" t="s">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="C11">
-        <x:v>6.31040096282959</x:v>
+        <x:v>7.490267276763916</x:v>
       </x:c>
       <x:c r="D11" t="s">
-        <x:v>22</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="E11" t="s">
-        <x:v>10</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="12">
-      <x:c r="A12">
-        <x:v>-4.6066741943359375</x:v>
-      </x:c>
-      <x:c r="B12" t="s">
-        <x:v>23</x:v>
-      </x:c>
-      <x:c r="C12">
-        <x:v>6.480711936950684</x:v>
-      </x:c>
-      <x:c r="D12" t="s">
-        <x:v>24</x:v>
-      </x:c>
-      <x:c r="E12" t="s">
-        <x:v>10</x:v>
+      <x:c r="F12" t="s">
+        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="13">
-      <x:c r="A13">
-        <x:v>-5.8532633781433105</x:v>
-      </x:c>
-      <x:c r="B13" t="s">
-        <x:v>25</x:v>
-      </x:c>
-      <x:c r="C13">
-        <x:v>4.184118270874023</x:v>
-      </x:c>
-      <x:c r="D13" t="s">
+      <x:c r="F13" t="s">
         <x:v>26</x:v>
-      </x:c>
-      <x:c r="E13" t="s">
-        <x:v>10</x:v>
       </x:c>
     </x:row>
     <x:row r="14">
@@ -696,12 +678,12 @@
       </x:c>
     </x:row>
     <x:row r="17">
-      <x:c r="F17" t="s">
+      <x:c r="G17" t="s">
         <x:v>30</x:v>
       </x:c>
     </x:row>
     <x:row r="18">
-      <x:c r="F18" t="s">
+      <x:c r="G18" t="s">
         <x:v>31</x:v>
       </x:c>
     </x:row>
@@ -711,8 +693,18 @@
       </x:c>
     </x:row>
     <x:row r="20">
-      <x:c r="H20" t="s">
+      <x:c r="G20" t="s">
         <x:v>33</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21">
+      <x:c r="G21" t="s">
+        <x:v>34</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22">
+      <x:c r="H22" t="s">
+        <x:v>35</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>